<commit_message>
Update flux metadata and attributes
</commit_message>
<xml_diff>
--- a/meta-data/flux_metadata_10min.xlsx
+++ b/meta-data/flux_metadata_10min.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33810DE6-59FD-CD43-930F-6DE4F508DC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E06C4C-B114-0F45-A4EF-AFDF90F05E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16660" yWindow="500" windowWidth="17620" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,9 +184,6 @@
     <t>Flux components and statistical quality checks.</t>
   </si>
   <si>
-    <t>0 m a.s.l</t>
-  </si>
-  <si>
     <t>sea ice</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">20 Hz sampling rate on both licor and sonic. Runs 10 mins in length. Run time stamp: start of run. </t>
+  </si>
+  <si>
+    <t>2 m a.s.l</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -679,7 +679,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -751,7 +751,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -772,10 +772,10 @@
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -783,7 +783,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -791,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -845,7 +845,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -861,7 +861,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -885,7 +885,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -946,7 +946,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -954,7 +954,7 @@
         <v>38</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -962,7 +962,7 @@
         <v>39</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>